<commit_message>
add all HD pairs
</commit_message>
<xml_diff>
--- a/pairwise_HD.xlsx
+++ b/pairwise_HD.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="17">
   <si>
     <t>Kazatzakis</t>
   </si>
@@ -55,15 +55,55 @@
   <si>
     <t>Voss</t>
   </si>
+  <si>
+    <t>Perseus-13</t>
+  </si>
+  <si>
+    <t>Kazatzakis-13</t>
+  </si>
+  <si>
+    <t>Polylas-13</t>
+  </si>
+  <si>
+    <t>Butler-13</t>
+  </si>
+  <si>
+    <t>Murray-13</t>
+  </si>
+  <si>
+    <t>Chapman-13</t>
+  </si>
+  <si>
+    <t>Pope-13</t>
+  </si>
+  <si>
+    <t>Voss-13</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -98,8 +138,100 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -108,7 +240,99 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="93">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -191,14 +415,14 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                   <c15:fullRef>
-                    <c15:sqref>Sheet1!$A$2:$B$9</c15:sqref>
+                    <c15:sqref>Sheet1!$A$1:$B$8</c15:sqref>
                   </c15:fullRef>
                   <c15:levelRef>
-                    <c15:sqref>Sheet1!$B$2:$B$9</c15:sqref>
+                    <c15:sqref>Sheet1!$B$1:$B$8</c15:sqref>
                   </c15:levelRef>
                 </c:ext>
               </c:extLst>
-              <c:f>Sheet1!$B$2:$B$9</c:f>
+              <c:f>Sheet1!$B$1:$B$8</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -230,7 +454,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$9</c:f>
+              <c:f>Sheet1!$C$1:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -272,11 +496,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-504383600"/>
-        <c:axId val="-485490416"/>
+        <c:axId val="-665711104"/>
+        <c:axId val="-665709056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-504383600"/>
+        <c:axId val="-665711104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -319,7 +543,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-485490416"/>
+        <c:crossAx val="-665709056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -327,7 +551,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-485490416"/>
+        <c:axId val="-665709056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -378,7 +602,851 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-504383600"/>
+        <c:crossAx val="-665711104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$9:$B$16</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="8"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Kazatzakis</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Pallis</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Polylas</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Butler</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Murray</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Pope</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Chapman</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Voss</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Perseus</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Kazatzakis-13</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Kazatzakis</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Kazatzakis</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Kazatzakis</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Kazatzakis</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Kazatzakis</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Kazatzakis</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$9:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.1043304</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.07968881</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.08521189</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.09090438</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.08302312</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.09924354</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.06866834</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0785646</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-609883248"/>
+        <c:axId val="-609863664"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-609883248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-609863664"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-609863664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-609883248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$1:$B$30</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="30"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Pallis</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Polylas</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Kazatzakis</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Butler</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Murray</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Pope</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Chapman</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Voss</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Kazatzakis</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Pallis</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Polylas</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>Butler</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Murray</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>Pope</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>Chapman</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>Voss</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>Butler</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>Murray</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>Pope</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>Chapman</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>Voss</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>Murray</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>Pope</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>Chapman</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>Voss</c:v>
+                  </c:pt>
+                  <c:pt idx="25">
+                    <c:v>Pope</c:v>
+                  </c:pt>
+                  <c:pt idx="26">
+                    <c:v>Chapman</c:v>
+                  </c:pt>
+                  <c:pt idx="27">
+                    <c:v>Voss</c:v>
+                  </c:pt>
+                  <c:pt idx="28">
+                    <c:v>Chapman</c:v>
+                  </c:pt>
+                  <c:pt idx="29">
+                    <c:v>Voss</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Perseus-13</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Perseus</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Perseus</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Perseus</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Perseus</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Perseus</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Perseus</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Perseus</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Perseus</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Kazatzakis-13</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Kazatzakis</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>Kazatzakis</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Kazatzakis</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>Kazatzakis</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>Kazatzakis</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>Kazatzakis</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>Polylas</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>Polylas</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>Polylas</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>Polylas</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>Polylas</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>Butler</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>Butler</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>Butler</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>Butler</c:v>
+                  </c:pt>
+                  <c:pt idx="25">
+                    <c:v>Murray</c:v>
+                  </c:pt>
+                  <c:pt idx="26">
+                    <c:v>Murray</c:v>
+                  </c:pt>
+                  <c:pt idx="27">
+                    <c:v>Murray</c:v>
+                  </c:pt>
+                  <c:pt idx="28">
+                    <c:v>Pope</c:v>
+                  </c:pt>
+                  <c:pt idx="29">
+                    <c:v>Pope</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$1:$C$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>0.02478207</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.02886676</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1043304</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.02683417</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.02792867</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.03091329</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.04566536</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.02152945</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.1043304</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.07968881</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.08521189</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.09090438</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.08302312</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.09924354</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.06866834</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.0785646</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.02721987</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.03154215</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.02103965</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.02406251</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.02545254</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.02012966</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.01884076</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.02806379</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.01545918</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.03098968</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.03524105</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.01412592</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.02361385</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.02246821</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-608990048"/>
+        <c:axId val="-609086848"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-608990048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-609086848"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-609086848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-608990048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -467,6 +1535,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -970,20 +2118,1026 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>182880</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>125431</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>325120</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>40640</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>721234</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>27595</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -997,6 +3151,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>253999</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>196301</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>341802</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>85921</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>338666</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>541866</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>169333</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1268,45 +3482,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C9"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="81" zoomScalePageLayoutView="81" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2.478207E-2</v>
+      </c>
+    </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1">
-        <v>2.478207E-2</v>
+        <v>2.8866760000000002E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2.8866760000000002E-2</v>
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.1043304</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.1043304</v>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2.6834170000000001E-2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1314,10 +3544,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C5" s="3">
-        <v>2.6834170000000001E-2</v>
+        <v>2.7928669999999999E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1325,10 +3555,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" s="3">
-        <v>2.7928669999999999E-2</v>
+        <v>3.091329E-2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1336,32 +3566,449 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="3">
+        <v>4.5665360000000002E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2.1529449999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.1043304</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>7.9688809999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>8.5211889999999998E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>9.0904380000000007E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>8.3023120000000006E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C14">
+        <v>9.9243540000000005E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>6.8668339999999994E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>7.8564599999999998E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>2.721987E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>3.1542149999999998E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <v>2.103965E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <v>2.4062509999999999E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <v>2.5452539999999999E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>2.0129660000000001E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23">
+        <v>1.8840760000000002E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <v>2.8063790000000002E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <v>1.5459179999999999E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26">
+        <v>3.0989679999999999E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27">
+        <v>3.5241050000000003E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28">
+        <v>1.412592E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29">
+        <v>2.3613849999999999E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30">
+        <v>2.2468209999999999E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C39" s="1">
+        <v>2.478207E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C40" s="1">
+        <v>2.8866760000000002E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C41" s="2">
+        <v>0.1043304</v>
+      </c>
+      <c r="F41" t="s">
+        <v>4</v>
+      </c>
+      <c r="G41" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C42" s="3">
+        <v>2.6834170000000001E-2</v>
+      </c>
+      <c r="F42" t="s">
+        <v>4</v>
+      </c>
+      <c r="G42" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C43" s="3">
+        <v>2.7928669999999999E-2</v>
+      </c>
+      <c r="F43" t="s">
+        <v>4</v>
+      </c>
+      <c r="G43" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C44" s="3">
         <v>3.091329E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="3">
+      <c r="F44" t="s">
+        <v>4</v>
+      </c>
+      <c r="G44" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C45" s="3">
         <v>4.5665360000000002E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="4">
+      <c r="F45" t="s">
+        <v>4</v>
+      </c>
+      <c r="G45" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C46" s="4">
         <v>2.1529449999999999E-2</v>
+      </c>
+      <c r="F46" t="s">
+        <v>4</v>
+      </c>
+      <c r="G46" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C47" s="2">
+        <v>0.1043304</v>
+      </c>
+    </row>
+    <row r="48" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C48">
+        <v>7.9688809999999999E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C49">
+        <v>8.5211889999999998E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C50">
+        <v>9.0904380000000007E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C51">
+        <v>8.3023120000000006E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C52">
+        <v>9.9243540000000005E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C53">
+        <v>6.8668339999999994E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C54">
+        <v>7.8564599999999998E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C55">
+        <v>2.721987E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C56">
+        <v>3.1542149999999998E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C57">
+        <v>2.103965E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C58">
+        <v>2.4062509999999999E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C59">
+        <v>2.5452539999999999E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C60">
+        <v>2.0129660000000001E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C61">
+        <v>1.8840760000000002E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C62">
+        <v>2.8063790000000002E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C63">
+        <v>1.5459179999999999E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C64">
+        <v>3.0989679999999999E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C65">
+        <v>3.5241050000000003E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C66">
+        <v>1.412592E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C67">
+        <v>2.3613849999999999E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C68">
+        <v>2.2468209999999999E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
clean up excel file with pairwise HD values
</commit_message>
<xml_diff>
--- a/pairwise_HD.xlsx
+++ b/pairwise_HD.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="11">
   <si>
     <t>Kazatzakis</t>
   </si>
@@ -60,24 +60,6 @@
   </si>
   <si>
     <t>Kazatzakis-13</t>
-  </si>
-  <si>
-    <t>Polylas-13</t>
-  </si>
-  <si>
-    <t>Butler-13</t>
-  </si>
-  <si>
-    <t>Murray-13</t>
-  </si>
-  <si>
-    <t>Chapman-13</t>
-  </si>
-  <si>
-    <t>Pope-13</t>
-  </si>
-  <si>
-    <t>Voss-13</t>
   </si>
 </sst>
 </file>
@@ -233,12 +215,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="93">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -496,11 +479,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-665711104"/>
-        <c:axId val="-665709056"/>
+        <c:axId val="1654103920"/>
+        <c:axId val="1654106240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-665711104"/>
+        <c:axId val="1654103920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -543,7 +526,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-665709056"/>
+        <c:crossAx val="1654106240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -551,7 +534,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-665709056"/>
+        <c:axId val="1654106240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -602,7 +585,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-665711104"/>
+        <c:crossAx val="1654103920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -718,41 +701,38 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$9:$B$16</c:f>
+              <c:f>Sheet1!$A$9:$B$15</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>Kazatzakis</c:v>
+                    <c:v>Pallis</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>Pallis</c:v>
+                    <c:v>Polylas</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>Polylas</c:v>
+                    <c:v>Butler</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>Butler</c:v>
+                    <c:v>Murray</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>Murray</c:v>
+                    <c:v>Pope</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>Pope</c:v>
+                    <c:v>Chapman</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>Chapman</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
                     <c:v>Voss</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>Perseus</c:v>
+                    <c:v>Kazatzakis-13</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>Kazatzakis-13</c:v>
+                    <c:v>Kazatzakis</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>Kazatzakis</c:v>
@@ -767,9 +747,6 @@
                     <c:v>Kazatzakis</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>Kazatzakis</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
                     <c:v>Kazatzakis</c:v>
                   </c:pt>
                 </c:lvl>
@@ -778,32 +755,29 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$9:$C$16</c:f>
+              <c:f>Sheet1!$C$9:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.1043304</c:v>
+                  <c:v>0.07968881</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.07968881</c:v>
+                  <c:v>0.08521189</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.08521189</c:v>
+                  <c:v>0.09090438</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.09090438</c:v>
+                  <c:v>0.08302312</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.08302312</c:v>
+                  <c:v>0.09924354</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.09924354</c:v>
+                  <c:v>0.06866834</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.06866834</c:v>
-                </c:pt>
-                <c:pt idx="7">
                   <c:v>0.0785646</c:v>
                 </c:pt>
               </c:numCache>
@@ -820,11 +794,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-609883248"/>
-        <c:axId val="-609863664"/>
+        <c:axId val="1654236416"/>
+        <c:axId val="1541336032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-609883248"/>
+        <c:axId val="1654236416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -867,7 +841,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-609863664"/>
+        <c:crossAx val="1541336032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -875,7 +849,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-609863664"/>
+        <c:axId val="1541336032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -925,7 +899,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-609883248"/>
+        <c:crossAx val="1654236416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1041,9 +1015,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$1:$B$30</c:f>
+              <c:f>Sheet1!$A$1:$B$29</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="30"/>
+                <c:ptCount val="29"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Pallis</c:v>
@@ -1070,69 +1044,66 @@
                     <c:v>Voss</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>Kazatzakis</c:v>
+                    <c:v>Pallis</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>Pallis</c:v>
+                    <c:v>Polylas</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>Polylas</c:v>
+                    <c:v>Butler</c:v>
                   </c:pt>
                   <c:pt idx="11">
+                    <c:v>Murray</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Pope</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>Chapman</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>Voss</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
                     <c:v>Butler</c:v>
                   </c:pt>
-                  <c:pt idx="12">
+                  <c:pt idx="16">
                     <c:v>Murray</c:v>
                   </c:pt>
-                  <c:pt idx="13">
+                  <c:pt idx="17">
                     <c:v>Pope</c:v>
                   </c:pt>
-                  <c:pt idx="14">
+                  <c:pt idx="18">
                     <c:v>Chapman</c:v>
                   </c:pt>
-                  <c:pt idx="15">
+                  <c:pt idx="19">
                     <c:v>Voss</c:v>
                   </c:pt>
-                  <c:pt idx="16">
-                    <c:v>Butler</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
+                  <c:pt idx="20">
                     <c:v>Murray</c:v>
                   </c:pt>
-                  <c:pt idx="18">
+                  <c:pt idx="21">
                     <c:v>Pope</c:v>
                   </c:pt>
-                  <c:pt idx="19">
+                  <c:pt idx="22">
                     <c:v>Chapman</c:v>
                   </c:pt>
-                  <c:pt idx="20">
+                  <c:pt idx="23">
                     <c:v>Voss</c:v>
                   </c:pt>
-                  <c:pt idx="21">
-                    <c:v>Murray</c:v>
-                  </c:pt>
-                  <c:pt idx="22">
+                  <c:pt idx="24">
                     <c:v>Pope</c:v>
                   </c:pt>
-                  <c:pt idx="23">
+                  <c:pt idx="25">
                     <c:v>Chapman</c:v>
                   </c:pt>
-                  <c:pt idx="24">
+                  <c:pt idx="26">
                     <c:v>Voss</c:v>
                   </c:pt>
-                  <c:pt idx="25">
-                    <c:v>Pope</c:v>
-                  </c:pt>
-                  <c:pt idx="26">
+                  <c:pt idx="27">
                     <c:v>Chapman</c:v>
                   </c:pt>
-                  <c:pt idx="27">
-                    <c:v>Voss</c:v>
-                  </c:pt>
                   <c:pt idx="28">
-                    <c:v>Chapman</c:v>
-                  </c:pt>
-                  <c:pt idx="29">
                     <c:v>Voss</c:v>
                   </c:pt>
                 </c:lvl>
@@ -1162,10 +1133,10 @@
                     <c:v>Perseus</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>Perseus</c:v>
+                    <c:v>Kazatzakis-13</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>Kazatzakis-13</c:v>
+                    <c:v>Kazatzakis</c:v>
                   </c:pt>
                   <c:pt idx="10">
                     <c:v>Kazatzakis</c:v>
@@ -1183,7 +1154,7 @@
                     <c:v>Kazatzakis</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>Kazatzakis</c:v>
+                    <c:v>Polylas</c:v>
                   </c:pt>
                   <c:pt idx="16">
                     <c:v>Polylas</c:v>
@@ -1198,7 +1169,7 @@
                     <c:v>Polylas</c:v>
                   </c:pt>
                   <c:pt idx="20">
-                    <c:v>Polylas</c:v>
+                    <c:v>Butler</c:v>
                   </c:pt>
                   <c:pt idx="21">
                     <c:v>Butler</c:v>
@@ -1210,7 +1181,7 @@
                     <c:v>Butler</c:v>
                   </c:pt>
                   <c:pt idx="24">
-                    <c:v>Butler</c:v>
+                    <c:v>Murray</c:v>
                   </c:pt>
                   <c:pt idx="25">
                     <c:v>Murray</c:v>
@@ -1219,12 +1190,9 @@
                     <c:v>Murray</c:v>
                   </c:pt>
                   <c:pt idx="27">
-                    <c:v>Murray</c:v>
+                    <c:v>Pope</c:v>
                   </c:pt>
                   <c:pt idx="28">
-                    <c:v>Pope</c:v>
-                  </c:pt>
-                  <c:pt idx="29">
                     <c:v>Pope</c:v>
                   </c:pt>
                 </c:lvl>
@@ -1233,10 +1201,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$1:$C$30</c:f>
+              <c:f>Sheet1!$C$1:$C$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>0.02478207</c:v>
                 </c:pt>
@@ -1262,69 +1230,66 @@
                   <c:v>0.02152945</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.1043304</c:v>
+                  <c:v>0.07968881</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.07968881</c:v>
+                  <c:v>0.08521189</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.08521189</c:v>
+                  <c:v>0.09090438</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.09090438</c:v>
+                  <c:v>0.08302312</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.08302312</c:v>
+                  <c:v>0.09924354</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.09924354</c:v>
+                  <c:v>0.06866834</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.06866834</c:v>
+                  <c:v>0.0785646</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.0785646</c:v>
+                  <c:v>0.02721987</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.02721987</c:v>
+                  <c:v>0.03154215</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.03154215</c:v>
+                  <c:v>0.02103965</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.02103965</c:v>
+                  <c:v>0.02406251</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.02406251</c:v>
+                  <c:v>0.02545254</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.02545254</c:v>
+                  <c:v>0.02012966</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.02012966</c:v>
+                  <c:v>0.01884076</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.01884076</c:v>
+                  <c:v>0.02806379</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.02806379</c:v>
+                  <c:v>0.01545918</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.01545918</c:v>
+                  <c:v>0.03098968</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.03098968</c:v>
+                  <c:v>0.03524105</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.03524105</c:v>
+                  <c:v>0.01412592</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.01412592</c:v>
+                  <c:v>0.02361385</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.02361385</c:v>
-                </c:pt>
-                <c:pt idx="29">
                   <c:v>0.02246821</c:v>
                 </c:pt>
               </c:numCache>
@@ -1341,11 +1306,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-608990048"/>
-        <c:axId val="-609086848"/>
+        <c:axId val="1541377984"/>
+        <c:axId val="1540974816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-608990048"/>
+        <c:axId val="1541377984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1388,7 +1353,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-609086848"/>
+        <c:crossAx val="1540974816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1396,7 +1361,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-609086848"/>
+        <c:axId val="1540974816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1446,7 +1411,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-608990048"/>
+        <c:crossAx val="1541377984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3482,10 +3447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="81" zoomScalePageLayoutView="81" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3584,25 +3549,25 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0.1043304</v>
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>7.9688809999999999E-2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10">
-        <v>7.9688809999999999E-2</v>
+        <v>8.5211889999999998E-2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -3610,10 +3575,10 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11">
-        <v>8.5211889999999998E-2</v>
+        <v>9.0904380000000007E-2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -3621,10 +3586,10 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C12">
-        <v>9.0904380000000007E-2</v>
+        <v>8.3023120000000006E-2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -3632,10 +3597,10 @@
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C13">
-        <v>8.3023120000000006E-2</v>
+        <v>9.9243540000000005E-2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -3643,10 +3608,10 @@
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C14">
-        <v>9.9243540000000005E-2</v>
+        <v>6.8668339999999994E-2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -3654,21 +3619,21 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C15">
-        <v>6.8668339999999994E-2</v>
+        <v>7.8564599999999998E-2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C16">
-        <v>7.8564599999999998E-2</v>
+        <v>2.721987E-2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -3676,10 +3641,10 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C17">
-        <v>2.721987E-2</v>
+        <v>3.1542149999999998E-2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -3687,10 +3652,10 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C18">
-        <v>3.1542149999999998E-2</v>
+        <v>2.103965E-2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -3698,10 +3663,10 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C19">
-        <v>2.103965E-2</v>
+        <v>2.4062509999999999E-2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -3709,21 +3674,21 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C20">
-        <v>2.4062509999999999E-2</v>
+        <v>2.5452539999999999E-2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C21">
-        <v>2.5452539999999999E-2</v>
+        <v>2.0129660000000001E-2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -3731,10 +3696,10 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C22">
-        <v>2.0129660000000001E-2</v>
+        <v>1.8840760000000002E-2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -3742,10 +3707,10 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C23">
-        <v>1.8840760000000002E-2</v>
+        <v>2.8063790000000002E-2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -3753,21 +3718,21 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C24">
-        <v>2.8063790000000002E-2</v>
+        <v>1.5459179999999999E-2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C25">
-        <v>1.5459179999999999E-2</v>
+        <v>3.0989679999999999E-2</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -3775,10 +3740,10 @@
         <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C26">
-        <v>3.0989679999999999E-2</v>
+        <v>3.5241050000000003E-2</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -3786,21 +3751,21 @@
         <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C27">
-        <v>3.5241050000000003E-2</v>
+        <v>1.412592E-2</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C28">
-        <v>1.412592E-2</v>
+        <v>2.3613849999999999E-2</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -3808,208 +3773,41 @@
         <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C29">
-        <v>2.3613849999999999E-2</v>
+        <v>2.2468209999999999E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>6</v>
-      </c>
-      <c r="B30" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30">
-        <v>2.2468209999999999E-2</v>
-      </c>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C39" s="1"/>
     </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C39" s="1">
-        <v>2.478207E-2</v>
-      </c>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C40" s="1"/>
     </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C40" s="1">
-        <v>2.8866760000000002E-2</v>
-      </c>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C41" s="4"/>
     </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C41" s="2">
-        <v>0.1043304</v>
-      </c>
-      <c r="F41" t="s">
-        <v>4</v>
-      </c>
-      <c r="G41" t="s">
-        <v>11</v>
-      </c>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C42" s="4"/>
     </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C42" s="3">
-        <v>2.6834170000000001E-2</v>
-      </c>
-      <c r="F42" t="s">
-        <v>4</v>
-      </c>
-      <c r="G42" t="s">
-        <v>12</v>
-      </c>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C43" s="4"/>
     </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C43" s="3">
-        <v>2.7928669999999999E-2</v>
-      </c>
-      <c r="F43" t="s">
-        <v>4</v>
-      </c>
-      <c r="G43" t="s">
-        <v>13</v>
-      </c>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C44" s="4"/>
     </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C44" s="3">
-        <v>3.091329E-2</v>
-      </c>
-      <c r="F44" t="s">
-        <v>4</v>
-      </c>
-      <c r="G44" t="s">
-        <v>15</v>
-      </c>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C45" s="4"/>
     </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C45" s="3">
-        <v>4.5665360000000002E-2</v>
-      </c>
-      <c r="F45" t="s">
-        <v>4</v>
-      </c>
-      <c r="G45" t="s">
-        <v>14</v>
-      </c>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C46" s="4"/>
     </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C46" s="4">
-        <v>2.1529449999999999E-2</v>
-      </c>
-      <c r="F46" t="s">
-        <v>4</v>
-      </c>
-      <c r="G46" t="s">
-        <v>16</v>
-      </c>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C47" s="4"/>
     </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C47" s="2">
-        <v>0.1043304</v>
-      </c>
-    </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C48">
-        <v>7.9688809999999999E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C49">
-        <v>8.5211889999999998E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C50">
-        <v>9.0904380000000007E-2</v>
-      </c>
-    </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C51">
-        <v>8.3023120000000006E-2</v>
-      </c>
-    </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C52">
-        <v>9.9243540000000005E-2</v>
-      </c>
-    </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C53">
-        <v>6.8668339999999994E-2</v>
-      </c>
-    </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C54">
-        <v>7.8564599999999998E-2</v>
-      </c>
-    </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C55">
-        <v>2.721987E-2</v>
-      </c>
-    </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C56">
-        <v>3.1542149999999998E-2</v>
-      </c>
-    </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C57">
-        <v>2.103965E-2</v>
-      </c>
-    </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C58">
-        <v>2.4062509999999999E-2</v>
-      </c>
-    </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C59">
-        <v>2.5452539999999999E-2</v>
-      </c>
-    </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C60">
-        <v>2.0129660000000001E-2</v>
-      </c>
-    </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C61">
-        <v>1.8840760000000002E-2</v>
-      </c>
-    </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C62">
-        <v>2.8063790000000002E-2</v>
-      </c>
-    </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C63">
-        <v>1.5459179999999999E-2</v>
-      </c>
-    </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C64">
-        <v>3.0989679999999999E-2</v>
-      </c>
-    </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C65">
-        <v>3.5241050000000003E-2</v>
-      </c>
-    </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C66">
-        <v>1.412592E-2</v>
-      </c>
-    </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C67">
-        <v>2.3613849999999999E-2</v>
-      </c>
-    </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C68">
-        <v>2.2468209999999999E-2</v>
-      </c>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C48" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>